<commit_message>
Updated the risk tracker with more risks
Renamed some of the risk types
</commit_message>
<xml_diff>
--- a/Risks/Project Risk Tracker.xlsx
+++ b/Risks/Project Risk Tracker.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="48" windowWidth="17052" windowHeight="11700"/>
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Risk Lists'!$B$2:$F$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Risk Lists'!$B$2:$G$16</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>Rank</t>
   </si>
@@ -48,63 +48,6 @@
     <t>A feasibility study will be conducted to verify compatible phone penetration rates, and if needed, we can tailor our platform to target only a certain segment of the customer base that has access to the required technology.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Technical Risks </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>- A technical malfunction of our platform might cause boarding delays for passengers and cause inefficiencies in LA Metro operations.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Partnership Risks</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> - The LA Metro might not be willing to implement our system or work with our group to test our platform on their systems/hardware.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Security Risks </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>- An unsecure platform might be exploited or easily manipulated (e.g. people finding loopholes to avoid fees), which can result in the LA Metro losing profits.</t>
-    </r>
-  </si>
-  <si>
     <t>Our group’s architect will develop a cryptosystem for our application that will be tested until it meets the client’s requirements and security standards.</t>
   </si>
   <si>
@@ -114,74 +57,87 @@
     <t>A back-up system will be designed in a later stage of the project. Also, we will advise passengers who are particularly sensitive to delays to have a back-up physical tap card.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Timing and Unexpected Risks -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> To get the application fully working and integrated into the LA Metro system, there will be a large set of evolving requirements. Two semesters might not be enough time to complete the project, especially if there are unexpected risks (e.g. another developer completes the same project before we do, bureaucratic risks, etc.)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>End-User Risks -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> End users (passengers) might not have smartphones that have the technical capabilities to support our platform.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Dynamic Risks -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> After the platform has been implemented and integrated, the LA Metro requirements might change, or the technologies being used in relevant processes might change.</t>
-    </r>
-  </si>
-  <si>
     <t>If we are under a contract/agreement, the team will develop updates/patches that will adapt to new requirements. Otherwise, we will give the LA Metro a copy of our comprehensive documentation for the software so that necessary changes can be handled in-house.</t>
   </si>
   <si>
     <t>Top Project Risks as of 09/16/2013</t>
+  </si>
+  <si>
+    <t>Identify team member skills and project requirements so we can individually prepare ourselves for technologies that we will be implementing next semester.</t>
+  </si>
+  <si>
+    <t>End users (passengers) might not have smartphones that have the technical capabilities to support our platform.</t>
+  </si>
+  <si>
+    <t>Risk Type</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>An unsecure platform might be exploited or easily manipulated (e.g. people finding loopholes to avoid fees), which can result in the LA Metro losing profits.</t>
+  </si>
+  <si>
+    <t>Partnership</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Estimation</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>People</t>
+  </si>
+  <si>
+    <t>The LA Metro might not be willing to implement our system or work with our group to test our platform on their systems/hardware.</t>
+  </si>
+  <si>
+    <t>To get the application fully working and integrated into the LA Metro system, there will be a large set of evolving requirements. Two semesters might not be enough time to complete the project, especially if there are unexpected risks (e.g. another developer completes the same project before we do, bureaucratic risks, etc.)</t>
+  </si>
+  <si>
+    <t>After the platform has been implemented and integrated, the LA Metro requirements might change, or the technologies being used in relevant processes might change.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Due to rapid formation of teams without proper analysis of required skill sets needed for this project we may lack the technical skills to complete this project in a professionally acceptable manner.
+</t>
+  </si>
+  <si>
+    <t>A technical malfunction of our platform might cause boarding delays for passengers and cause inefficiencies in LA Metro operations.</t>
+  </si>
+  <si>
+    <t>Tools</t>
+  </si>
+  <si>
+    <t>We will be using PhoneGap to implement the mobile application with standard web technologies like HTML/CSS/Javascript which makes the application subject to device-specific mobile browser display discrepencies.</t>
+  </si>
+  <si>
+    <t>Test on a wide variety of devices (different iPhone versions and various Android phones) to ensure the application is rendered properly on all screen sizes and OS versions.</t>
+  </si>
+  <si>
+    <t>Organizational</t>
+  </si>
+  <si>
+    <t>The statically defined list of team roles may not fit our specific project requirements.</t>
+  </si>
+  <si>
+    <t>Dynamically reassign team roles as the project and its requirements mature.  Also the team shall be aware that responsibilities will be very flexible and we may need to step outside the scope of our assigned position</t>
+  </si>
+  <si>
+    <t>The amount of cooperation needed between our team and LA Metro may be more than expected which could make this project unfeasible for them.</t>
+  </si>
+  <si>
+    <t>Come up with a plan focused around the idea that LA Metro should have to do as little as possible.  Extensive testing should be done internally before our software can be ready for LA Metro.  The goal should be to get it right the first time.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +179,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -232,7 +196,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -457,11 +421,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -491,9 +466,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -506,7 +478,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -545,19 +526,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -861,232 +855,304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.88671875" customWidth="1"/>
-    <col min="4" max="4" width="40.5546875" customWidth="1"/>
-    <col min="5" max="5" width="50.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="40.5546875" customWidth="1"/>
+    <col min="6" max="6" width="50.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="19"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="22"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="22"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="24"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="22"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="24"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="F5" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="G5" s="29" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="28"/>
       <c r="F6" s="28"/>
-    </row>
-    <row r="7" spans="2:6" ht="36" x14ac:dyDescent="0.3">
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" spans="1:7" ht="36" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="31">
+      <c r="D7" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="36" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <f>B7+1</f>
         <v>2</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="31">
+      <c r="G8" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="36" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <f t="shared" ref="B9:B16" si="0">B8+1</f>
         <v>3</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="31">
+      <c r="D9" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="36" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="D10" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="33">
+      <c r="G10" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="84" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
-        <f t="shared" si="0"/>
+        <f>B10+1</f>
         <v>5</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="6" t="s">
+      <c r="D11" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="7">
+      <c r="G11" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="48.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="7">
+      <c r="D12" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="4">
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.3">
+      <c r="A13" s="32"/>
+      <c r="B13" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="48" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="12">
+      <c r="C15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="53.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
+      <c r="C16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="40">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B2:F4"/>
+  <mergeCells count="6">
+    <mergeCell ref="B2:G4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="D5:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="93" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="88" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>